<commit_message>
2 flow temp version xl
</commit_message>
<xml_diff>
--- a/radiator calculator.xlsx
+++ b/radiator calculator.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\phili\Documents\GitSourceCode\Radiators\radiators2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF5E4016-5E57-4B06-9C34-91463BBACCD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49F66E9C-3791-4C1A-8B8F-5E96D6B9D57D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="43560" yWindow="495" windowWidth="26655" windowHeight="14430" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,17 +16,15 @@
     <sheet name="Summary" sheetId="10" r:id="rId1"/>
     <sheet name="RadiatorDatabase" sheetId="2" r:id="rId2"/>
     <sheet name="Rooms" sheetId="9" r:id="rId3"/>
-    <sheet name="test" sheetId="11" r:id="rId4"/>
-    <sheet name="Examples" sheetId="6" r:id="rId5"/>
-    <sheet name="Design" sheetId="7" r:id="rId6"/>
-    <sheet name="Tabular" sheetId="3" r:id="rId7"/>
-    <sheet name="Form" sheetId="13" r:id="rId8"/>
-    <sheet name="RadReplacementStrategy" sheetId="14" r:id="rId9"/>
+    <sheet name="Examples" sheetId="6" r:id="rId4"/>
+    <sheet name="Design" sheetId="7" r:id="rId5"/>
+    <sheet name="Tabular" sheetId="3" r:id="rId6"/>
+    <sheet name="Form" sheetId="13" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="FlowRateScenario">Table5[#All]</definedName>
     <definedName name="LabourCosts">Table4[#All]</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="7">Form!$A:$G</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="6">Form!$A:$G</definedName>
     <definedName name="RoomEmittersMaxSizes">Table3[#All]</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -64,7 +62,7 @@
       </extLst>
     </bk>
   </futureMetadata>
-  <futureMetadata name="XLRICHVALUE" count="3">
+  <futureMetadata name="XLRICHVALUE" count="5">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -75,7 +73,14 @@
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
-          <xlrd:rvb i="4"/>
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="5"/>
         </ext>
       </extLst>
     </bk>
@@ -86,13 +91,20 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="8"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
   <cellMetadata count="1">
     <bk>
       <rc t="1" v="0"/>
     </bk>
   </cellMetadata>
-  <valueMetadata count="3">
+  <valueMetadata count="5">
     <bk>
       <rc t="2" v="0"/>
     </bk>
@@ -101,6 +113,12 @@
     </bk>
     <bk>
       <rc t="2" v="2"/>
+    </bk>
+    <bk>
+      <rc t="2" v="3"/>
+    </bk>
+    <bk>
+      <rc t="2" v="4"/>
     </bk>
   </valueMetadata>
 </metadata>
@@ -368,9 +386,7 @@
  </code>
     </pythonScript>
     <pythonScript>
-      <code xml:space="preserve">
-#=======================================================================================================
-def load_dataframes_from_excel():
+      <code xml:space="preserve">def load_dataframes_from_excel():
     rad_db = xl(%P2%, headers=True)
     rooms = xl(%P3%, headers=True)
     max_sizes = xl(%P4%, headers=True)
@@ -379,19 +395,17 @@
     return rad_db, rooms, max_sizes, labour_costs, flow_rate_scenario
 rad_db, rooms, max_sizes, labour_costs, flow_rate_scenario = load_dataframes_from_excel()
 home = Home(rooms, max_sizes, rad_db)
-flow_temperature = xl(%P7%)
-print("Got here")
-results = home.minimal_cost_radiators(flow_temperature)
-print("And here")
-results
 </code>
+    </pythonScript>
+    <pythonScript>
+      <code>home.minimal_cost_radiators(xl(%P2%))</code>
     </pythonScript>
   </pythonScripts>
 </python>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="110">
   <si>
     <t>K1</t>
   </si>
@@ -675,165 +689,6 @@
     <t>FlowRate</t>
   </si>
   <si>
-    <t>Rad @ 55FT</t>
-  </si>
-  <si>
-    <t>Rad @ 50FT</t>
-  </si>
-  <si>
-    <t>Rad @ 45FT</t>
-  </si>
-  <si>
-    <t>Rad @ 40FT</t>
-  </si>
-  <si>
-    <t>Rad @ 35FT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                645.9536480916148
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                451.3802466347125
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                360.54416027213864
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                274.7317341310722
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                194.74573581005535
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x600x450:
-                NA-
-                £68.5-
-                £50-
-                121.79964487125997
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                2447.2460203519504
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                1710.0894398627383
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                1365.9498076895848
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                1040.8427059789587
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                737.8094826922875
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x1800x600:
-                NA-
-                £198.04-
-                £50-
-                461.4475002534491
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                942.787110202426
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                677.1898584697104
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                552.4770508290045
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                433.97182213418563
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                322.545224837744
-                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">ModernxK2x800x450:
-                NA-
-                £79.19-
-                £50-
-                219.4441586125635
-                </t>
-  </si>
-  <si>
     <t>Condition</t>
   </si>
   <si>
@@ -841,39 +696,6 @@
   </si>
   <si>
     <t>ModernxK2x1200x600</t>
-  </si>
-  <si>
-    <t>Existing Rad 1</t>
-  </si>
-  <si>
-    <t>Space 1</t>
-  </si>
-  <si>
-    <t>1000W £50</t>
-  </si>
-  <si>
-    <t>2000W £400</t>
-  </si>
-  <si>
-    <t>500W £60</t>
-  </si>
-  <si>
-    <t>1200W £40</t>
-  </si>
-  <si>
-    <t>4000W £400</t>
-  </si>
-  <si>
-    <t>Loop through this rad 1st</t>
-  </si>
-  <si>
-    <t>Find Rad 2 which has &gt; W`</t>
-  </si>
-  <si>
-    <t>Existing Rad 2</t>
-  </si>
-  <si>
-    <t>Find Space 1 with &gt; W or zero</t>
   </si>
   <si>
     <t>Depth</t>
@@ -910,6 +732,9 @@
   </si>
   <si>
     <t>Loc3</t>
+  </si>
+  <si>
+    <t>Load Tables</t>
   </si>
 </sst>
 </file>
@@ -1328,8 +1153,8 @@
 </file>
 
 <file path=xl/richData/rdarray.xml><?xml version="1.0" encoding="utf-8"?>
-<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="1">
-  <a r="5" c="9">
+<arrayData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" count="2">
+  <a r="7" c="9">
     <v t="s"/>
     <v t="s">Room Name</v>
     <v t="s">Location name</v>
@@ -1370,17 +1195,100 @@
     <v t="s">Dining</v>
     <v t="s">Loc1</v>
     <v t="s">ModernxK2x800x450</v>
+    <v t="s">ModernxK2x1400x600</v>
+    <v>154.06</v>
+    <v>95</v>
+    <v t="s">Replaced</v>
+    <v>1114.7647804363507</v>
+    <v>4</v>
+    <v t="s">Bed 1</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x800x450</v>
     <v t="s">ModernxK2x1200x600</v>
     <v>119.57</v>
     <v>95</v>
     <v t="s">Replaced</v>
-    <v>955.24998505020085</v>
+    <v>1046.5335566296003</v>
+    <v>5</v>
+    <v t="s">Bath 1</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x800x450</v>
+    <v t="s">ModernxK2x1400x600</v>
+    <v>154.06</v>
+    <v>95</v>
+    <v t="s">Replaced</v>
+    <v>1010.538750674492</v>
+  </a>
+  <a r="7" c="9">
+    <v t="s"/>
+    <v t="s">Room Name</v>
+    <v t="s">Location name</v>
+    <v t="s">Originally</v>
+    <v t="s">Proposed Radiator</v>
+    <v t="s">£</v>
+    <v t="s">Labour Cost</v>
+    <v t="s">Status</v>
+    <v t="s">Watts</v>
+    <v>0</v>
+    <v t="s">Lounge</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x600x450</v>
+    <v t="s">ModernxK2x600x450</v>
+    <v>0</v>
+    <v>0</v>
+    <v t="s">Original</v>
+    <v>194.74573581005535</v>
+    <v>1</v>
+    <v t="s">Lounge</v>
+    <v t="s">Loc2</v>
+    <v t="s">ModernxK2x1200x600</v>
+    <v t="s">ModernxK2x1200x600</v>
+    <v>0</v>
+    <v>0</v>
+    <v t="s">Original</v>
+    <v>491.71523573911912</v>
+    <v>2</v>
+    <v t="s">Lounge</v>
+    <v t="s">Loc3</v>
+    <v t="r">0</v>
+    <v t="s">ModernxK2x1200x700</v>
+    <v>198.48</v>
+    <v>300</v>
+    <v t="s">Replaced</v>
+    <v>556.78823373154341</v>
+    <v>3</v>
+    <v t="s">Dining</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x800x450</v>
+    <v t="s">ModernxK3x1800x600</v>
+    <v>469</v>
+    <v>95</v>
+    <v t="s">Replaced</v>
+    <v>1098.3908672589328</v>
+    <v>4</v>
+    <v t="s">Bed 1</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x800x450</v>
+    <v t="s">ModernxK2x2000x600</v>
+    <v>303.12</v>
+    <v>95</v>
+    <v t="s">Replaced</v>
+    <v>1018.5019679470787</v>
+    <v>5</v>
+    <v t="s">Bath 1</v>
+    <v t="s">Loc1</v>
+    <v t="s">ModernxK2x800x450</v>
+    <v t="s">ModernxK2x2000x600</v>
+    <v>303.12</v>
+    <v>95</v>
+    <v t="s">Replaced</v>
+    <v>755.697673733648</v>
   </a>
 </arrayData>
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="9">
   <rv s="0">
     <fb>0</fb>
     <v>0</v>
@@ -1394,12 +1302,18 @@
     <v>1</v>
   </rv>
   <rv s="2">
+    <v>&lt;class '__main__.Home'&gt;</v>
+    <v>Home</v>
+    <v>&lt;__main__.Home object at 0x7f32eb341340&gt;</v>
+    <v>1</v>
+  </rv>
+  <rv s="3">
     <v>0</v>
   </rv>
-  <rv s="3">
+  <rv s="4">
     <v>DataFrame</v>
     <v>3</v>
-    <v>2</v>
+    <v>3</v>
   </rv>
   <rv s="1">
     <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
@@ -1408,14 +1322,32 @@
 0    Lounge          Loc1   ModernxK2x600x450   ModernxK2x600x450    0.00   
 1    Lounge          Loc2  ModernxK2x1200x600  ModernxK2x1200x600    0.00   
 2    Lounge          ...</v>
+    <v>4</v>
+    <v>1</v>
+  </rv>
+  <rv s="3">
+    <v>1</v>
+  </rv>
+  <rv s="4">
+    <v>DataFrame</v>
     <v>3</v>
+    <v>6</v>
+  </rv>
+  <rv s="1">
+    <v>&lt;class 'pandas.core.frame.DataFrame'&gt;</v>
+    <v>DataFrame</v>
+    <v xml:space="preserve">  Room Name Location name          Originally   Proposed Radiator       £  \
+0    Lounge          Loc1   ModernxK2x600x450   ModernxK2x600x450    0.00   
+1    Lounge          Loc2  ModernxK2x1200x600  ModernxK2x1200x600    0.00   
+2    Lounge          ...</v>
+    <v>7</v>
     <v>1</v>
   </rv>
 </rvData>
 </file>
 
 <file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
-<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="4">
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="5">
   <s t="_formattednumber">
     <k n="_Format" t="spb"/>
   </s>
@@ -1424,6 +1356,12 @@
     <k n="Python_typeName" t="s"/>
     <k n="Python_str" t="s"/>
     <k n="preview" t="r"/>
+    <k n="_Provider" t="spb"/>
+  </s>
+  <s t="_python">
+    <k n="Python_type" t="s"/>
+    <k n="Python_typeName" t="s"/>
+    <k n="Python_str" t="s"/>
     <k n="_Provider" t="spb"/>
   </s>
   <s t="_array">
@@ -1449,7 +1387,7 @@
       <v>Python provided by Anaconda</v>
     </spb>
     <spb s="2">
-      <v>4</v>
+      <v>6</v>
       <v>8</v>
       <v>DataFrame</v>
       <v>arrayPreview</v>
@@ -1533,8 +1471,8 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{570897E6-0B07-42F1-B411-FB58D6817A44}" name="Table3" displayName="Table3" ref="E1:M5" totalsRowShown="0">
-  <autoFilter ref="E1:M5" xr:uid="{570897E6-0B07-42F1-B411-FB58D6817A44}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{570897E6-0B07-42F1-B411-FB58D6817A44}" name="Table3" displayName="Table3" ref="E1:M7" totalsRowShown="0">
+  <autoFilter ref="E1:M7" xr:uid="{570897E6-0B07-42F1-B411-FB58D6817A44}"/>
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{D800A84A-07CB-4911-96AE-EAFD0F8CAE30}" name="Room Name"/>
     <tableColumn id="10" xr3:uid="{CF65C992-0CA1-4F09-9DED-4750959DD52A}" name="Location"/>
@@ -1551,8 +1489,8 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{617FE319-FEA4-4FD1-9A4E-11D892AB84BD}" name="Table4" displayName="Table4" ref="E14:F18" totalsRowShown="0">
-  <autoFilter ref="E14:F18" xr:uid="{617FE319-FEA4-4FD1-9A4E-11D892AB84BD}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{617FE319-FEA4-4FD1-9A4E-11D892AB84BD}" name="Table4" displayName="Table4" ref="P1:Q5" totalsRowShown="0">
+  <autoFilter ref="P1:Q5" xr:uid="{617FE319-FEA4-4FD1-9A4E-11D892AB84BD}"/>
   <tableColumns count="2">
     <tableColumn id="1" xr3:uid="{ECF6E62E-BB01-4FD4-839D-CAB76FE7AFEA}" name="Labour Type"/>
     <tableColumn id="2" xr3:uid="{19D99575-9A42-46DE-85F3-BFB8A4F67596}" name="Cost" dataDxfId="0"/>
@@ -1876,13 +1814,13 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>98</v>
       </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
       <c r="C1" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="D1" t="s">
         <v>4</v>
@@ -6046,10 +5984,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A28468E-1C96-4244-AAD3-D4DE1A24BCD5}">
-  <dimension ref="A1:S34"/>
+  <dimension ref="A1:S52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A38" sqref="A38:XFD41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6074,13 +6012,13 @@
         <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>133</v>
+        <v>99</v>
       </c>
       <c r="E1" t="s">
         <v>70</v>
       </c>
       <c r="F1" t="s">
-        <v>139</v>
+        <v>105</v>
       </c>
       <c r="G1" t="s">
         <v>7</v>
@@ -6092,16 +6030,22 @@
         <v>3</v>
       </c>
       <c r="J1" t="s">
-        <v>131</v>
+        <v>97</v>
       </c>
       <c r="K1" t="s">
-        <v>134</v>
+        <v>100</v>
       </c>
       <c r="L1" t="s">
         <v>75</v>
       </c>
       <c r="M1" t="s">
         <v>76</v>
+      </c>
+      <c r="P1" t="s">
+        <v>86</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>85</v>
       </c>
       <c r="S1" t="s">
         <v>76</v>
@@ -6121,7 +6065,7 @@
         <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="G2">
         <v>1200</v>
@@ -6143,6 +6087,12 @@
       </c>
       <c r="M2" t="s">
         <v>78</v>
+      </c>
+      <c r="P2" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q2" s="1">
+        <v>50</v>
       </c>
       <c r="S2" t="s">
         <v>77</v>
@@ -6162,7 +6112,7 @@
         <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
       <c r="G3">
         <v>2000</v>
@@ -6177,13 +6127,19 @@
         <v>2</v>
       </c>
       <c r="K3">
-        <v>300</v>
+        <v>95</v>
       </c>
       <c r="L3" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="M3" t="s">
         <v>79</v>
+      </c>
+      <c r="P3" t="s">
+        <v>88</v>
+      </c>
+      <c r="Q3" s="1">
+        <v>100</v>
       </c>
       <c r="S3" t="s">
         <v>78</v>
@@ -6203,7 +6159,7 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>142</v>
+        <v>108</v>
       </c>
       <c r="G4">
         <v>1200</v>
@@ -6218,10 +6174,16 @@
         <v>8</v>
       </c>
       <c r="K4">
-        <v>95</v>
+        <v>300</v>
       </c>
       <c r="M4" t="s">
         <v>81</v>
+      </c>
+      <c r="P4" t="s">
+        <v>89</v>
+      </c>
+      <c r="Q4" s="1">
+        <v>250</v>
       </c>
       <c r="S4" t="s">
         <v>79</v>
@@ -6241,10 +6203,10 @@
         <v>18</v>
       </c>
       <c r="F5" t="s">
-        <v>140</v>
+        <v>106</v>
       </c>
       <c r="G5">
-        <v>1200</v>
+        <v>2000</v>
       </c>
       <c r="H5">
         <v>600</v>
@@ -6253,7 +6215,7 @@
         <v>73</v>
       </c>
       <c r="J5" t="s">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="K5">
         <v>95</v>
@@ -6264,8 +6226,72 @@
       <c r="M5" t="s">
         <v>79</v>
       </c>
+      <c r="P5" t="s">
+        <v>90</v>
+      </c>
+      <c r="Q5" s="1">
+        <v>10</v>
+      </c>
       <c r="S5" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="E6" t="s">
+        <v>71</v>
+      </c>
+      <c r="F6" t="s">
+        <v>106</v>
+      </c>
+      <c r="G6">
+        <v>2000</v>
+      </c>
+      <c r="H6">
+        <v>600</v>
+      </c>
+      <c r="I6" t="s">
+        <v>73</v>
+      </c>
+      <c r="J6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>95</v>
+      </c>
+      <c r="L6" t="s">
+        <v>82</v>
+      </c>
+      <c r="M6" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.45">
+      <c r="E7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F7" t="s">
+        <v>106</v>
+      </c>
+      <c r="G7">
+        <v>2000</v>
+      </c>
+      <c r="H7">
+        <v>600</v>
+      </c>
+      <c r="I7" t="s">
+        <v>73</v>
+      </c>
+      <c r="J7" t="s">
+        <v>2</v>
+      </c>
+      <c r="K7">
+        <v>95</v>
+      </c>
+      <c r="L7" t="s">
+        <v>82</v>
+      </c>
+      <c r="M7" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.45">
@@ -6273,12 +6299,6 @@
       <c r="J10" s="1"/>
     </row>
     <row r="14" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="E14" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" t="s">
-        <v>85</v>
-      </c>
       <c r="H14" t="s">
         <v>92</v>
       </c>
@@ -6287,12 +6307,6 @@
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="E15" t="s">
-        <v>87</v>
-      </c>
-      <c r="F15" s="1">
-        <v>50</v>
-      </c>
       <c r="H15" t="s">
         <v>91</v>
       </c>
@@ -6301,12 +6315,6 @@
       </c>
     </row>
     <row r="16" spans="1:19" x14ac:dyDescent="0.45">
-      <c r="E16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F16" s="1">
-        <v>100</v>
-      </c>
       <c r="H16" t="str">
         <f>"Rad @ "&amp;I16&amp;"FT"</f>
         <v>Rad @ 55FT</v>
@@ -6316,12 +6324,6 @@
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="E17" t="s">
-        <v>89</v>
-      </c>
-      <c r="F17" s="1">
-        <v>250</v>
-      </c>
       <c r="H17" t="str">
         <f>"Rad @ "&amp;I17&amp;"FT"</f>
         <v>Rad @ 50FT</v>
@@ -6331,12 +6333,6 @@
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" s="1">
-        <v>10</v>
-      </c>
       <c r="H18" t="str">
         <f>"Rad @ "&amp;I18&amp;"FT"</f>
         <v>Rad @ 45FT</v>
@@ -6365,7 +6361,7 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>135</v>
+        <v>101</v>
       </c>
       <c r="B25" cm="1" vm="1">
         <f t="array" ref="B25">_xlfn._xlws.PY(0,1)</f>
@@ -6374,7 +6370,7 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>136</v>
+        <v>102</v>
       </c>
       <c r="B26" cm="1" vm="1">
         <f t="array" ref="B26">_xlfn._xlws.PY(1,1)</f>
@@ -6383,7 +6379,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>137</v>
+        <v>103</v>
       </c>
       <c r="B27" cm="1" vm="1">
         <f t="array" ref="B27">_xlfn._xlws.PY(2,1)</f>
@@ -6392,94 +6388,74 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>138</v>
+        <v>104</v>
       </c>
       <c r="B28" cm="1" vm="1">
         <f t="array" ref="B28">_xlfn._xlws.PY(3,1)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A30" t="e" cm="1" vm="2">
-        <f t="array" ref="A30">_xlfn._xlws.PY(4,1,RadiatorDatabase[#All],Rooms[#All],RoomEmittersMaxSizes,LabourCosts,FlowRateScenario,A31)</f>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A29" t="s">
+        <v>109</v>
+      </c>
+      <c r="B29" t="e" cm="1" vm="2">
+        <f t="array" ref="B29">_xlfn._xlws.PY(4,1,RadiatorDatabase[#All],Rooms[#All],RoomEmittersMaxSizes,LabourCosts,FlowRateScenario)</f>
         <v>#VALUE!</v>
       </c>
-      <c r="B30" t="str" cm="1">
-        <f t="array" ref="B30:J34">_FV(A30,"arrayPreview")</f>
-        <v/>
-      </c>
-      <c r="C30" t="str">
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A31" t="e" cm="1" vm="3">
+        <f t="array" ref="A31">_xlfn._xlws.PY(5,1,A32)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B31" t="str" cm="1">
+        <f t="array" ref="B31:J37">_FV(A31,"arrayPreview")</f>
+        <v/>
+      </c>
+      <c r="C31" t="str">
         <v>Room Name</v>
       </c>
-      <c r="D30" t="str">
+      <c r="D31" t="str">
         <v>Location name</v>
       </c>
-      <c r="E30" t="str">
+      <c r="E31" t="str">
         <v>Originally</v>
       </c>
-      <c r="F30" t="str">
+      <c r="F31" t="str">
         <v>Proposed Radiator</v>
       </c>
-      <c r="G30" t="str">
+      <c r="G31" t="str">
         <v>£</v>
       </c>
-      <c r="H30" t="str">
+      <c r="H31" t="str">
         <v>Labour Cost</v>
       </c>
-      <c r="I30" t="str">
+      <c r="I31" t="str">
         <v>Status</v>
       </c>
-      <c r="J30" t="str">
+      <c r="J31" t="str">
         <v>Watts</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="A31">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A32">
         <v>50</v>
       </c>
-      <c r="B31">
+      <c r="B32">
         <v>0</v>
-      </c>
-      <c r="C31" t="str">
-        <v>Lounge</v>
-      </c>
-      <c r="D31" t="str">
-        <v>Loc1</v>
-      </c>
-      <c r="E31" t="str">
-        <v>ModernxK2x600x450</v>
-      </c>
-      <c r="F31" t="str">
-        <v>ModernxK2x600x450</v>
-      </c>
-      <c r="G31">
-        <v>0</v>
-      </c>
-      <c r="H31">
-        <v>0</v>
-      </c>
-      <c r="I31" t="str">
-        <v>Original</v>
-      </c>
-      <c r="J31">
-        <v>360.54416027213864</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
-      <c r="B32">
-        <v>1</v>
       </c>
       <c r="C32" t="str">
         <v>Lounge</v>
       </c>
       <c r="D32" t="str">
-        <v>Loc2</v>
+        <v>Loc1</v>
       </c>
       <c r="E32" t="str">
-        <v>ModernxK2x1200x600</v>
+        <v>ModernxK2x600x450</v>
       </c>
       <c r="F32" t="str">
-        <v>ModernxK2x1200x600</v>
+        <v>ModernxK2x600x450</v>
       </c>
       <c r="G32">
         <v>0</v>
@@ -6491,24 +6467,24 @@
         <v>Original</v>
       </c>
       <c r="J32">
-        <v>910.34114829344355</v>
-      </c>
-    </row>
-    <row r="33" spans="2:10" x14ac:dyDescent="0.45">
+        <v>360.54416027213864</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.45">
       <c r="B33">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C33" t="str">
         <v>Lounge</v>
       </c>
       <c r="D33" t="str">
-        <v>Loc3</v>
-      </c>
-      <c r="E33" vm="3">
-        <v>0</v>
-      </c>
-      <c r="F33" vm="3">
-        <v>0</v>
+        <v>Loc2</v>
+      </c>
+      <c r="E33" t="str">
+        <v>ModernxK2x1200x600</v>
+      </c>
+      <c r="F33" t="str">
+        <v>ModernxK2x1200x600</v>
       </c>
       <c r="G33">
         <v>0</v>
@@ -6517,44 +6493,343 @@
         <v>0</v>
       </c>
       <c r="I33" t="str">
-        <v/>
+        <v>Original</v>
       </c>
       <c r="J33">
+        <v>910.34114829344355</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34" t="str">
+        <v>Lounge</v>
+      </c>
+      <c r="D34" t="str">
+        <v>Loc3</v>
+      </c>
+      <c r="E34" vm="4">
         <v>0</v>
       </c>
-    </row>
-    <row r="34" spans="2:10" x14ac:dyDescent="0.45">
-      <c r="B34">
+      <c r="F34" vm="4">
+        <v>0</v>
+      </c>
+      <c r="G34">
+        <v>0</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34" t="str">
+        <v/>
+      </c>
+      <c r="J34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B35">
         <v>3</v>
       </c>
-      <c r="C34" t="str">
+      <c r="C35" t="str">
         <v>Dining</v>
       </c>
-      <c r="D34" t="str">
+      <c r="D35" t="str">
         <v>Loc1</v>
       </c>
-      <c r="E34" t="str">
+      <c r="E35" t="str">
         <v>ModernxK2x800x450</v>
       </c>
-      <c r="F34" t="str">
+      <c r="F35" t="str">
+        <v>ModernxK2x1400x600</v>
+      </c>
+      <c r="G35">
+        <v>154.06</v>
+      </c>
+      <c r="H35">
+        <v>95</v>
+      </c>
+      <c r="I35" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J35">
+        <v>1114.7647804363507</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36" t="str">
+        <v>Bed 1</v>
+      </c>
+      <c r="D36" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E36" t="str">
+        <v>ModernxK2x800x450</v>
+      </c>
+      <c r="F36" t="str">
         <v>ModernxK2x1200x600</v>
       </c>
-      <c r="G34">
+      <c r="G36">
         <v>119.57</v>
       </c>
-      <c r="H34">
+      <c r="H36">
         <v>95</v>
       </c>
-      <c r="I34" t="str">
+      <c r="I36" t="str">
         <v>Replaced</v>
       </c>
-      <c r="J34">
-        <v>955.24998505020085</v>
+      <c r="J36">
+        <v>1046.5335566296003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37" t="str">
+        <v>Bath 1</v>
+      </c>
+      <c r="D37" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E37" t="str">
+        <v>ModernxK2x800x450</v>
+      </c>
+      <c r="F37" t="str">
+        <v>ModernxK2x1400x600</v>
+      </c>
+      <c r="G37">
+        <v>154.06</v>
+      </c>
+      <c r="H37">
+        <v>95</v>
+      </c>
+      <c r="I37" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J37">
+        <v>1010.538750674492</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A46" t="e" cm="1" vm="5">
+        <f t="array" ref="A46">_xlfn._xlws.PY(5,1,A47)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="B46" t="str" cm="1">
+        <f t="array" ref="B46:J52">_FV(A46,"arrayPreview")</f>
+        <v/>
+      </c>
+      <c r="C46" t="str">
+        <v>Room Name</v>
+      </c>
+      <c r="D46" t="str">
+        <v>Location name</v>
+      </c>
+      <c r="E46" t="str">
+        <v>Originally</v>
+      </c>
+      <c r="F46" t="str">
+        <v>Proposed Radiator</v>
+      </c>
+      <c r="G46" t="str">
+        <v>£</v>
+      </c>
+      <c r="H46" t="str">
+        <v>Labour Cost</v>
+      </c>
+      <c r="I46" t="str">
+        <v>Status</v>
+      </c>
+      <c r="J46" t="str">
+        <v>Watts</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="A47">
+        <v>40</v>
+      </c>
+      <c r="B47">
+        <v>0</v>
+      </c>
+      <c r="C47" t="str">
+        <v>Lounge</v>
+      </c>
+      <c r="D47" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E47" t="str">
+        <v>ModernxK2x600x450</v>
+      </c>
+      <c r="F47" t="str">
+        <v>ModernxK2x600x450</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47" t="str">
+        <v>Original</v>
+      </c>
+      <c r="J47">
+        <v>194.74573581005535</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="B48">
+        <v>1</v>
+      </c>
+      <c r="C48" t="str">
+        <v>Lounge</v>
+      </c>
+      <c r="D48" t="str">
+        <v>Loc2</v>
+      </c>
+      <c r="E48" t="str">
+        <v>ModernxK2x1200x600</v>
+      </c>
+      <c r="F48" t="str">
+        <v>ModernxK2x1200x600</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48" t="str">
+        <v>Original</v>
+      </c>
+      <c r="J48">
+        <v>491.71523573911912</v>
+      </c>
+    </row>
+    <row r="49" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B49">
+        <v>2</v>
+      </c>
+      <c r="C49" t="str">
+        <v>Lounge</v>
+      </c>
+      <c r="D49" t="str">
+        <v>Loc3</v>
+      </c>
+      <c r="E49" vm="4">
+        <v>0</v>
+      </c>
+      <c r="F49" t="str">
+        <v>ModernxK2x1200x700</v>
+      </c>
+      <c r="G49">
+        <v>198.48</v>
+      </c>
+      <c r="H49">
+        <v>300</v>
+      </c>
+      <c r="I49" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J49">
+        <v>556.78823373154341</v>
+      </c>
+    </row>
+    <row r="50" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50" t="str">
+        <v>Dining</v>
+      </c>
+      <c r="D50" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E50" t="str">
+        <v>ModernxK2x800x450</v>
+      </c>
+      <c r="F50" t="str">
+        <v>ModernxK3x1800x600</v>
+      </c>
+      <c r="G50">
+        <v>469</v>
+      </c>
+      <c r="H50">
+        <v>95</v>
+      </c>
+      <c r="I50" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J50">
+        <v>1098.3908672589328</v>
+      </c>
+    </row>
+    <row r="51" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B51">
+        <v>4</v>
+      </c>
+      <c r="C51" t="str">
+        <v>Bed 1</v>
+      </c>
+      <c r="D51" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E51" t="str">
+        <v>ModernxK2x800x450</v>
+      </c>
+      <c r="F51" t="str">
+        <v>ModernxK2x2000x600</v>
+      </c>
+      <c r="G51">
+        <v>303.12</v>
+      </c>
+      <c r="H51">
+        <v>95</v>
+      </c>
+      <c r="I51" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J51">
+        <v>1018.5019679470787</v>
+      </c>
+    </row>
+    <row r="52" spans="2:10" x14ac:dyDescent="0.45">
+      <c r="B52">
+        <v>5</v>
+      </c>
+      <c r="C52" t="str">
+        <v>Bath 1</v>
+      </c>
+      <c r="D52" t="str">
+        <v>Loc1</v>
+      </c>
+      <c r="E52" t="str">
+        <v>ModernxK2x800x450</v>
+      </c>
+      <c r="F52" t="str">
+        <v>ModernxK2x2000x600</v>
+      </c>
+      <c r="G52">
+        <v>303.12</v>
+      </c>
+      <c r="H52">
+        <v>95</v>
+      </c>
+      <c r="I52" t="str">
+        <v>Replaced</v>
+      </c>
+      <c r="J52">
+        <v>755.697673733648</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M5" xr:uid="{D7A455FC-3304-487E-A662-A1B935170611}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="M2:M7" xr:uid="{D7A455FC-3304-487E-A662-A1B935170611}">
       <formula1>$S$2:$S$5</formula1>
     </dataValidation>
   </dataValidations>
@@ -6573,19 +6848,19 @@
           <x14:formula1>
             <xm:f>'RadiatorDatabase'!$L$2:$L$2</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I5</xm:sqref>
+          <xm:sqref>I2:I7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{293B7A05-DF40-4A48-B853-65447368AE4F}">
           <x14:formula1>
             <xm:f>'RadiatorDatabase'!$M$2:$M$5</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J5</xm:sqref>
+          <xm:sqref>J2:J7</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{65890CA2-F1A7-4285-A48C-25F54E1662B9}">
           <x14:formula1>
             <xm:f>'RadiatorDatabase'!$A$2:$A$147</xm:f>
           </x14:formula1>
-          <xm:sqref>L2:L5</xm:sqref>
+          <xm:sqref>L2:L7</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -6594,174 +6869,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A880353D-53C7-4C36-B4B6-BAC4AE71C690}">
-  <dimension ref="A1:I5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="4" max="4" width="71.33203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>70</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>91</v>
-      </c>
-      <c r="E1" t="s">
-        <v>94</v>
-      </c>
-      <c r="F1" t="s">
-        <v>95</v>
-      </c>
-      <c r="G1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H1" t="s">
-        <v>97</v>
-      </c>
-      <c r="I1" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2">
-        <v>1500</v>
-      </c>
-      <c r="C2">
-        <v>600</v>
-      </c>
-      <c r="D2" t="s">
-        <v>99</v>
-      </c>
-      <c r="E2" t="s">
-        <v>100</v>
-      </c>
-      <c r="F2" t="s">
-        <v>101</v>
-      </c>
-      <c r="G2" t="s">
-        <v>102</v>
-      </c>
-      <c r="H2" t="s">
-        <v>103</v>
-      </c>
-      <c r="I2" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3">
-        <v>2000</v>
-      </c>
-      <c r="C3">
-        <v>900</v>
-      </c>
-      <c r="D3" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" t="s">
-        <v>106</v>
-      </c>
-      <c r="F3" t="s">
-        <v>107</v>
-      </c>
-      <c r="G3" t="s">
-        <v>108</v>
-      </c>
-      <c r="H3" t="s">
-        <v>109</v>
-      </c>
-      <c r="I3" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
-      </c>
-      <c r="C4">
-        <v>200</v>
-      </c>
-      <c r="D4">
-        <v>0</v>
-      </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>18</v>
-      </c>
-      <c r="B5">
-        <v>2000</v>
-      </c>
-      <c r="C5">
-        <v>100</v>
-      </c>
-      <c r="D5" t="s">
-        <v>111</v>
-      </c>
-      <c r="E5" t="s">
-        <v>112</v>
-      </c>
-      <c r="F5" t="s">
-        <v>113</v>
-      </c>
-      <c r="G5" t="s">
-        <v>114</v>
-      </c>
-      <c r="H5" t="s">
-        <v>115</v>
-      </c>
-      <c r="I5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B481CD40-786D-47C7-B7F7-34323C25509A}">
   <dimension ref="O17:O18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M1" sqref="M1:S16"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6783,7 +6895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{816285A1-A71E-447E-BA79-2ABEB518C2CD}">
   <dimension ref="A1:H30"/>
   <sheetViews>
@@ -7369,7 +7481,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D269F0-F0FA-4CCF-8FCF-84BE210D1C1D}">
   <dimension ref="A1:S68"/>
   <sheetViews>
@@ -11321,7 +11433,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40D4B4CD-8DDF-40B2-A157-38E8306B97DE}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
@@ -11363,7 +11475,7 @@
         <v>75</v>
       </c>
       <c r="G1" s="24" t="s">
-        <v>117</v>
+        <v>94</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.45">
@@ -11386,7 +11498,7 @@
         <v>80</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.45">
@@ -11777,67 +11889,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" scale="98" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{045F260C-F26F-4A55-9C09-C31113677A50}">
-  <dimension ref="A2:G4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="4" max="4" width="12.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>120</v>
-      </c>
-      <c r="B2" t="s">
-        <v>122</v>
-      </c>
-      <c r="C2" t="s">
-        <v>123</v>
-      </c>
-      <c r="E2" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B3" t="s">
-        <v>124</v>
-      </c>
-      <c r="C3" t="s">
-        <v>125</v>
-      </c>
-      <c r="F3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" t="s">
-        <v>126</v>
-      </c>
-      <c r="C4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>